<commit_message>
Update dictionary curation logic
</commit_message>
<xml_diff>
--- a/input/dictionaries/conc_medium_dict.xlsx
+++ b/input/dictionaries/conc_medium_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\CvT Database\input\dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JWALL01\ONEDRI~1\Profile\DOCUME~1\MobaXterm\slash\RemoteFiles\66710_2_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD40C6-2E46-47F4-8AD3-DCF5C987D86E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948420F4-13E0-42F1-A120-894D78DEC94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="168" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>capillary blood</t>
-  </si>
-  <si>
-    <t>Capillary Blood</t>
   </si>
   <si>
     <t>fat (mesenteric)</t>
@@ -660,17 +657,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -692,13 +689,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -706,10 +703,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -720,10 +717,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -734,10 +731,10 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -748,10 +745,10 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -762,10 +759,10 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -776,10 +773,10 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -790,10 +787,10 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -804,10 +801,10 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -818,10 +815,10 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -832,10 +829,10 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -846,10 +843,10 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -860,10 +857,10 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -874,10 +871,10 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -888,10 +885,10 @@
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -899,13 +896,13 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -916,10 +913,10 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -927,13 +924,13 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -944,10 +941,10 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -958,10 +955,10 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -969,13 +966,13 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -986,10 +983,10 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1000,10 +997,10 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1014,10 +1011,10 @@
         <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1028,10 +1025,10 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1042,10 +1039,10 @@
         <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1056,10 +1053,10 @@
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1070,10 +1067,10 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1081,10 +1078,10 @@
         <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1095,10 +1092,10 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1109,10 +1106,10 @@
         <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1120,13 +1117,13 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1134,13 +1131,13 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1151,10 +1148,10 @@
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1165,10 +1162,10 @@
         <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1179,10 +1176,10 @@
         <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1193,10 +1190,10 @@
         <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1204,458 +1201,458 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
       </c>
       <c r="D45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="s">
         <v>54</v>
       </c>
-      <c r="C49" t="s">
-        <v>55</v>
-      </c>
       <c r="D49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
         <v>34</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
         <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
         <v>34</v>
       </c>
       <c r="D57" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
         <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
         <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
         <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" t="s">
         <v>34</v>
       </c>
       <c r="D64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
         <v>34</v>
       </c>
       <c r="D65" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" t="s">
         <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" t="s">
         <v>74</v>
       </c>
-      <c r="C68" t="s">
-        <v>75</v>
-      </c>
       <c r="D68" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" t="s">
         <v>76</v>
       </c>
-      <c r="C69" t="s">
-        <v>77</v>
-      </c>
       <c r="D69" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D70" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PFAS_PIP template dictionary updates
</commit_message>
<xml_diff>
--- a/input/dictionaries/conc_medium_dict.xlsx
+++ b/input/dictionaries/conc_medium_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7709CD-77E0-40C3-BD2C-B2CA6D1FAC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4F617D-63E4-4547-865B-ADE1B898317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2505" windowWidth="14010" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>venous blood</t>
+  </si>
+  <si>
+    <t>gastrocnemius</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,6 +2569,17 @@
         <v>44622.910884457713</v>
       </c>
     </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>90</v>
+      </c>
+      <c r="C73" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>